<commit_message>
Updated 1590b Schematic Rev 6
* Added a DNP SMD Resistor pad to optionally bypass the PDS1 isolated power components.
</commit_message>
<xml_diff>
--- a/Hardware/GuitarPedal1590b/docs/Bill_of_Materials_BOM.xlsx
+++ b/Hardware/GuitarPedal1590b/docs/Bill_of_Materials_BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/GuitarPedal1590b/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshep/Dev/DaisySeedProjects/Hardware/GuitarPedal1590b/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDDA797-78F8-8548-8D13-12D2A146F130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEA23F9-5AC2-A84E-9A84-997043234A66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38640" yWindow="960" windowWidth="25700" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1320" windowWidth="25700" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="116">
   <si>
     <t>Item #</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>Use two 20pin female headers to make a socket for the Seed.  This is needed since some components fit under the seed.  I used these: https://www.amazon.com/dp/B09MYBZZKZ</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>DNP (Do Not Place)</t>
   </si>
 </sst>
 </file>
@@ -902,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1556,58 +1562,46 @@
       <c r="A24" s="11">
         <v>22</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>9</v>
+      <c r="B24" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C24" s="11">
-        <v>1</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="16" t="s">
-        <v>102</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="11">
         <v>23</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C25" s="11">
         <v>1</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>76</v>
+        <v>100</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1615,28 +1609,28 @@
         <v>24</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="C26" s="11">
         <v>1</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1644,28 +1638,28 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C27" s="11">
         <v>1</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>106</v>
+        <v>77</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>107</v>
+        <v>84</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1673,48 +1667,66 @@
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="C28" s="11">
         <v>1</v>
       </c>
       <c r="D28" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="11">
+        <v>27</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="11">
+        <v>1</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E29" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F29" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G29" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="16" t="s">
+      <c r="H29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="14"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
+      <c r="I30" s="14"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="11"/>
@@ -1870,18 +1882,29 @@
       <c r="H44" s="11"/>
       <c r="I44" s="12"/>
     </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="11"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="12"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I12" r:id="rId1" xr:uid="{0EAF0846-CD42-354F-AECF-2172BB70C45D}"/>
     <hyperlink ref="I11" r:id="rId2" xr:uid="{EC151C2C-77B9-5C41-BAC9-D2A63F75EE6E}"/>
     <hyperlink ref="I4" r:id="rId3" xr:uid="{F9DB8EE7-AC99-3C47-8FA1-A700B0977DF6}"/>
-    <hyperlink ref="I24" r:id="rId4" xr:uid="{66BB8C28-609F-DE40-B04D-CF31C217E668}"/>
-    <hyperlink ref="I25" r:id="rId5" xr:uid="{CCEFA8AE-B5E5-B542-9A94-05C6EE0386BE}"/>
-    <hyperlink ref="I26" r:id="rId6" xr:uid="{04AAC3D9-518F-DF43-8D9F-500C377B974E}"/>
-    <hyperlink ref="I27" r:id="rId7" xr:uid="{10210211-C02A-6242-A06D-257B5BEDBBF9}"/>
+    <hyperlink ref="I25" r:id="rId4" xr:uid="{66BB8C28-609F-DE40-B04D-CF31C217E668}"/>
+    <hyperlink ref="I26" r:id="rId5" xr:uid="{CCEFA8AE-B5E5-B542-9A94-05C6EE0386BE}"/>
+    <hyperlink ref="I27" r:id="rId6" xr:uid="{04AAC3D9-518F-DF43-8D9F-500C377B974E}"/>
+    <hyperlink ref="I28" r:id="rId7" xr:uid="{10210211-C02A-6242-A06D-257B5BEDBBF9}"/>
     <hyperlink ref="I10" r:id="rId8" xr:uid="{3A50486B-EFB8-3C42-A260-36061CEC7211}"/>
     <hyperlink ref="D10" r:id="rId9" display="https://www.mouser.com/manufacturer/gravitech/" xr:uid="{3F61889C-263C-3546-B96A-848C4B005F30}"/>
-    <hyperlink ref="I28" r:id="rId10" xr:uid="{F25F2715-BF35-C14D-AAA9-AF45B9818986}"/>
+    <hyperlink ref="I29" r:id="rId10" xr:uid="{F25F2715-BF35-C14D-AAA9-AF45B9818986}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>

</xml_diff>